<commit_message>
Update file - model evaluation file
</commit_message>
<xml_diff>
--- a/file/모델 평가 정리.xlsx
+++ b/file/모델 평가 정리.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18075" windowHeight="11295"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18075" windowHeight="11265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.0000"/>
+    <numFmt numFmtId="176" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +119,23 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -129,18 +146,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -148,6 +153,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,13 +411,223 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -410,14 +637,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -428,17 +664,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -446,233 +706,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -695,16 +757,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>668609</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>156881</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>321227</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>201705</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>257736</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>146469</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>191293</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -728,7 +790,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8904933" y="7664822"/>
+          <a:off x="13342462" y="7496734"/>
           <a:ext cx="4374038" cy="2757441"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -750,16 +812,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>655544</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>30757</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>196103</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>131611</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>395313</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>44823</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>313765</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>170656</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -783,8 +845,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8891868" y="2428816"/>
-          <a:ext cx="4524680" cy="2781919"/>
+          <a:off x="13217338" y="2103846"/>
+          <a:ext cx="4219015" cy="2593986"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -805,16 +867,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>246529</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22413</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>145678</xdr:rowOff>
+      <xdr:rowOff>22414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>615033</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>390917</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>145677</xdr:rowOff>
+      <xdr:rowOff>22413</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -838,8 +900,503 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4381500" y="7653619"/>
+          <a:off x="8942295" y="7530355"/>
           <a:ext cx="4469857" cy="2767852"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>61033</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>270192</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8953500" y="4801121"/>
+          <a:ext cx="4337927" cy="2751644"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>33619</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>112060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>207880</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8953501" y="2084295"/>
+          <a:ext cx="4275614" cy="2666999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>145677</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>67237</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>466389</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="145677" y="2039472"/>
+          <a:ext cx="4455683" cy="2767852"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123266</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>67237</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>379228</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="123266" y="4807325"/>
+          <a:ext cx="4390933" cy="2723028"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>32519</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="그림 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="89647" y="7540460"/>
+          <a:ext cx="4403912" cy="2744860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>78442</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>18183</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4628030" y="2050677"/>
+          <a:ext cx="4310035" cy="2711823"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>425824</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>112060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>677043</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="그림 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4560795" y="4852148"/>
+          <a:ext cx="4352572" cy="2689411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>437030</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>11207</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>192072</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="그림 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4572001" y="7541558"/>
+          <a:ext cx="4359088" cy="2713396"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>280147</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>416133</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>112060</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="그림 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13301382" y="4751294"/>
+          <a:ext cx="4237339" cy="2655795"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1126,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1139,34 +1696,34 @@
   <sheetData>
     <row r="1" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="72"/>
+      <c r="C2" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="29" t="s">
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="50" t="s">
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="52"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="83"/>
       <c r="V2" s="70" t="s">
         <v>16</v>
       </c>
@@ -1177,395 +1734,455 @@
       <c r="AA2" s="71"/>
     </row>
     <row r="3" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="11" t="s">
+      <c r="B3" s="73"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="34" t="s">
+      <c r="L3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="33" t="s">
+      <c r="N3" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="34" t="s">
+      <c r="O3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="53" t="s">
+      <c r="P3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="54" t="s">
+      <c r="T3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="55" t="s">
+      <c r="U3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="53" t="s">
+      <c r="V3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="54" t="s">
+      <c r="Z3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="V3" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="W3" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="X3" s="74" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y3" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z3" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA3" s="74" t="s">
+      <c r="AA3" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="55">
         <v>3371</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17">
-        <v>6140</v>
-      </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="35">
+      <c r="E4" s="84"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="33">
+        <v>5115</v>
+      </c>
+      <c r="H4" s="84"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="56">
         <v>5686</v>
       </c>
-      <c r="K4" s="36"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="38">
-        <v>8254</v>
-      </c>
-      <c r="N4" s="36"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="56">
+      <c r="K4" s="90"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="44">
+        <v>8512</v>
+      </c>
+      <c r="N4" s="90"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="8">
         <v>118</v>
       </c>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="58"/>
+      <c r="Q4" s="96"/>
+      <c r="R4" s="97"/>
       <c r="S4" s="59">
-        <v>76</v>
-      </c>
-      <c r="T4" s="57"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="75">
+        <v>113</v>
+      </c>
+      <c r="T4" s="96"/>
+      <c r="U4" s="97"/>
+      <c r="V4" s="18">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="W4" s="76"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="78">
+      <c r="W4" s="102"/>
+      <c r="X4" s="103"/>
+      <c r="Y4" s="19">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Z4" s="76"/>
-      <c r="AA4" s="77"/>
+      <c r="Z4" s="102"/>
+      <c r="AA4" s="103"/>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B5" s="4"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="74"/>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="34">
         <v>3482</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21">
-        <v>2371</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="39">
+      <c r="E5" s="86"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="53">
+        <v>3291</v>
+      </c>
+      <c r="H5" s="86"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="57">
         <v>6027</v>
       </c>
-      <c r="K5" s="40"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="42">
-        <v>5449</v>
-      </c>
-      <c r="N5" s="40"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="60">
+      <c r="K5" s="92"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="46">
+        <v>6721</v>
+      </c>
+      <c r="N5" s="92"/>
+      <c r="O5" s="93"/>
+      <c r="P5" s="9">
         <v>225</v>
       </c>
-      <c r="Q5" s="61"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="63">
-        <v>312</v>
-      </c>
-      <c r="T5" s="61"/>
-      <c r="U5" s="62"/>
-      <c r="V5" s="79">
+      <c r="Q5" s="98"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="60">
+        <v>111</v>
+      </c>
+      <c r="T5" s="98"/>
+      <c r="U5" s="99"/>
+      <c r="V5" s="20">
         <v>3.3E-3</v>
       </c>
-      <c r="W5" s="80"/>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="82">
+      <c r="W5" s="104"/>
+      <c r="X5" s="105"/>
+      <c r="Y5" s="21">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Z5" s="80"/>
-      <c r="AA5" s="81"/>
+      <c r="Z5" s="104"/>
+      <c r="AA5" s="105"/>
     </row>
     <row r="6" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="3"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="73"/>
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="52">
         <v>2830</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="21">
-        <v>1961</v>
-      </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="39">
+      <c r="E6" s="88"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="54">
+        <v>2985</v>
+      </c>
+      <c r="H6" s="88"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="45">
         <v>5810</v>
       </c>
-      <c r="K6" s="43"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="42">
-        <v>4669</v>
-      </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="64">
+      <c r="K6" s="94"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="58">
+        <v>5267</v>
+      </c>
+      <c r="N6" s="94"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="61">
         <v>95</v>
       </c>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="66"/>
-      <c r="S6" s="67">
-        <v>861</v>
-      </c>
-      <c r="T6" s="65"/>
-      <c r="U6" s="66"/>
-      <c r="V6" s="83">
+      <c r="Q6" s="100"/>
+      <c r="R6" s="101"/>
+      <c r="S6" s="12">
+        <v>143</v>
+      </c>
+      <c r="T6" s="100"/>
+      <c r="U6" s="101"/>
+      <c r="V6" s="22">
         <v>3.8E-3</v>
       </c>
-      <c r="W6" s="84"/>
-      <c r="X6" s="85"/>
-      <c r="Y6" s="86">
+      <c r="W6" s="106"/>
+      <c r="X6" s="107"/>
+      <c r="Y6" s="23">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="Z6" s="84"/>
-      <c r="AA6" s="85"/>
+      <c r="Z6" s="106"/>
+      <c r="AA6" s="107"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="55">
         <v>0.01</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="17">
+      <c r="E7" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="F7" s="36">
+        <v>0.02</v>
+      </c>
+      <c r="G7" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="H7" s="68">
         <v>0.01</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="24">
+      <c r="I7" s="36">
         <v>0.03</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7" s="56">
         <v>0.03</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="38">
+      <c r="K7" s="44">
+        <v>0.06</v>
+      </c>
+      <c r="L7" s="47">
+        <v>0.04</v>
+      </c>
+      <c r="M7" s="69">
         <v>0.03</v>
       </c>
-      <c r="N7" s="38"/>
-      <c r="O7" s="45">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="P7" s="60">
+      <c r="N7" s="44">
+        <v>0.04</v>
+      </c>
+      <c r="O7" s="47">
+        <v>0.05</v>
+      </c>
+      <c r="P7" s="9">
         <v>259</v>
       </c>
-      <c r="Q7" s="63"/>
-      <c r="R7" s="68"/>
+      <c r="Q7" s="60">
+        <v>66</v>
+      </c>
+      <c r="R7" s="64">
+        <v>220</v>
+      </c>
       <c r="S7" s="63">
-        <v>103</v>
-      </c>
-      <c r="T7" s="63"/>
-      <c r="U7" s="68">
-        <v>278</v>
-      </c>
-      <c r="V7" s="75">
+        <v>83</v>
+      </c>
+      <c r="T7" s="10">
+        <v>80</v>
+      </c>
+      <c r="U7" s="13">
+        <v>69</v>
+      </c>
+      <c r="V7" s="18">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="W7" s="87"/>
-      <c r="X7" s="88">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="87">
-        <v>2E-3</v>
-      </c>
-      <c r="Z7" s="87"/>
-      <c r="AA7" s="88">
-        <v>0</v>
+      <c r="W7" s="24">
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="X7" s="25">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="Y7" s="24">
+        <v>1.9E-3</v>
+      </c>
+      <c r="Z7" s="24">
+        <v>1.35E-2</v>
+      </c>
+      <c r="AA7" s="25">
+        <v>3.8999999999999998E-3</v>
       </c>
     </row>
     <row r="8" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="74"/>
+      <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="34">
         <v>0.01</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="21">
+      <c r="E8" s="35">
+        <v>0.02</v>
+      </c>
+      <c r="F8" s="37">
         <v>0.01</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="25">
+      <c r="G8" s="35">
+        <v>0.02</v>
+      </c>
+      <c r="H8" s="35">
+        <v>0.02</v>
+      </c>
+      <c r="I8" s="37">
         <v>0.01</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="45">
         <v>0.03</v>
       </c>
-      <c r="K8" s="42"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="42">
-        <v>0.03</v>
-      </c>
-      <c r="N8" s="42"/>
-      <c r="O8" s="46">
-        <v>0.03</v>
-      </c>
-      <c r="P8" s="60">
+      <c r="K8" s="46">
+        <v>0.04</v>
+      </c>
+      <c r="L8" s="48">
+        <v>0.04</v>
+      </c>
+      <c r="M8" s="46">
+        <v>0.04</v>
+      </c>
+      <c r="N8" s="46">
+        <v>0.04</v>
+      </c>
+      <c r="O8" s="48">
+        <v>0.04</v>
+      </c>
+      <c r="P8" s="62">
         <v>58</v>
       </c>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="68"/>
-      <c r="S8" s="63">
-        <v>65</v>
-      </c>
-      <c r="T8" s="63"/>
-      <c r="U8" s="68">
-        <v>65</v>
-      </c>
-      <c r="V8" s="83">
+      <c r="Q8" s="63">
+        <v>64</v>
+      </c>
+      <c r="R8" s="64">
+        <v>79</v>
+      </c>
+      <c r="S8" s="10">
+        <v>64</v>
+      </c>
+      <c r="T8" s="10">
+        <v>64</v>
+      </c>
+      <c r="U8" s="13">
+        <v>81</v>
+      </c>
+      <c r="V8" s="22">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="W8" s="86"/>
-      <c r="X8" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="86">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="Z8" s="86"/>
-      <c r="AA8" s="89">
-        <v>0</v>
+      <c r="W8" s="23">
+        <v>1.18E-2</v>
+      </c>
+      <c r="X8" s="26">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="Y8" s="21">
+        <v>1E-3</v>
+      </c>
+      <c r="Z8" s="23">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="AA8" s="26">
+        <v>3.3E-3</v>
       </c>
     </row>
     <row r="9" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="3"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="73"/>
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="38">
         <v>0.01</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28">
-        <v>0.02</v>
-      </c>
-      <c r="G9" s="27">
+      <c r="E9" s="39">
         <v>0.01</v>
       </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28">
-        <v>0.02</v>
-      </c>
-      <c r="J9" s="47">
+      <c r="F9" s="40">
+        <v>0.01</v>
+      </c>
+      <c r="G9" s="39">
+        <v>0.01</v>
+      </c>
+      <c r="H9" s="39">
+        <v>0.01</v>
+      </c>
+      <c r="I9" s="40">
+        <v>0.01</v>
+      </c>
+      <c r="J9" s="49">
         <v>0.03</v>
       </c>
-      <c r="K9" s="48"/>
-      <c r="L9" s="49">
-        <v>0.06</v>
-      </c>
-      <c r="M9" s="48">
+      <c r="K9" s="50">
+        <v>0.04</v>
+      </c>
+      <c r="L9" s="51">
+        <v>0.04</v>
+      </c>
+      <c r="M9" s="50">
         <v>0.03</v>
       </c>
-      <c r="N9" s="48"/>
-      <c r="O9" s="49">
-        <v>0.05</v>
-      </c>
-      <c r="P9" s="64">
+      <c r="N9" s="50">
+        <v>0.04</v>
+      </c>
+      <c r="O9" s="51">
+        <v>0.04</v>
+      </c>
+      <c r="P9" s="11">
         <v>324</v>
       </c>
-      <c r="Q9" s="67"/>
-      <c r="R9" s="69">
-        <v>78</v>
-      </c>
-      <c r="S9" s="67">
+      <c r="Q9" s="65">
         <v>61</v>
       </c>
-      <c r="T9" s="67"/>
-      <c r="U9" s="69">
-        <v>204</v>
-      </c>
-      <c r="V9" s="90">
+      <c r="R9" s="67">
+        <v>91</v>
+      </c>
+      <c r="S9" s="12">
+        <v>171</v>
+      </c>
+      <c r="T9" s="12">
+        <v>157</v>
+      </c>
+      <c r="U9" s="14">
+        <v>157</v>
+      </c>
+      <c r="V9" s="27">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="W9" s="91"/>
-      <c r="X9" s="92">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="91">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="Z9" s="91"/>
-      <c r="AA9" s="92">
-        <v>0</v>
+      <c r="W9" s="66">
+        <v>1.4E-2</v>
+      </c>
+      <c r="X9" s="29">
+        <v>3.8E-3</v>
+      </c>
+      <c r="Y9" s="28">
+        <v>1.8E-3</v>
+      </c>
+      <c r="Z9" s="28">
+        <v>1.21E-2</v>
+      </c>
+      <c r="AA9" s="29">
+        <v>1.1999999999999999E-3</v>
       </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.3">
@@ -1585,6 +2202,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="V2:AA2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="H4:I6"/>
     <mergeCell ref="N4:O6"/>
     <mergeCell ref="T4:U6"/>
@@ -1593,14 +2218,6 @@
     <mergeCell ref="K4:L6"/>
     <mergeCell ref="Q4:R6"/>
     <mergeCell ref="W4:X6"/>
-    <mergeCell ref="V2:AA2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update File - All Trainer
</commit_message>
<xml_diff>
--- a/file/모델 평가 정리.xlsx
+++ b/file/모델 평가 정리.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="21">
   <si>
     <t>Many-to-One</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +95,18 @@
     <t>모델</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Transformer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>확진자 예측</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIR 계수 예측</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -103,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,21 +132,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="KoPubWorld돋움체 Light"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="KoPubWorld돋움체 Light"/>
       <family val="3"/>
       <charset val="129"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="KoPubWorld돋움체 Light"/>
       <family val="3"/>
       <charset val="129"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -411,329 +429,350 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -759,14 +798,14 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>321227</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>201705</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>593912</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>191293</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>57943</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -814,14 +853,14 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>196103</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>131611</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>313765</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>170656</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>65881</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -869,14 +908,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>22413</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>22414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>390917</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>22413</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>127188</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -924,14 +963,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>33618</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>61033</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>270192</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>44824</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>149599</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -979,14 +1018,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>33619</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>112060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>207880</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>115981</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1034,14 +1073,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>145677</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>67237</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>466389</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>67236</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>172011</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1089,14 +1128,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>123266</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>67237</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>379228</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>127187</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1144,14 +1183,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>89647</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>32519</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1199,14 +1238,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>493059</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>78442</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>18183</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>127187</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1254,14 +1293,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>425824</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>112060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>677043</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>33618</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>138393</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1309,14 +1348,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>437030</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>33617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>11207</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>192072</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>87297</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1364,14 +1403,14 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>280147</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>11206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>416133</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>112060</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>7285</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1681,527 +1720,920 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AA14"/>
+  <dimension ref="B1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="8.125" customWidth="1"/>
+    <col min="1" max="1" width="3" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="72"/>
-      <c r="C2" s="72" t="s">
+    <row r="1" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="113" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="78" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="81" t="s">
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="83"/>
-      <c r="V2" s="70" t="s">
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
-      <c r="AA2" s="71"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="14"/>
     </row>
-    <row r="3" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="73"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="30" t="s">
+    <row r="3" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="114"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="41" t="s">
+      <c r="M3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="N3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="U3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="W3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="X3" s="17" t="s">
+      <c r="X3" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="Z3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="17" t="s">
+      <c r="AA3" s="28" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="55">
+      <c r="D4" s="30">
         <v>3371</v>
       </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="33">
         <v>5115</v>
       </c>
-      <c r="H4" s="84"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="56">
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="34">
         <v>5686</v>
       </c>
-      <c r="K4" s="90"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="44">
+      <c r="K4" s="35"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="37">
         <v>8512</v>
       </c>
-      <c r="N4" s="90"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="8">
+      <c r="N4" s="35"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="38">
         <v>118</v>
       </c>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="59">
+      <c r="Q4" s="39"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="41">
         <v>113</v>
       </c>
-      <c r="T4" s="96"/>
-      <c r="U4" s="97"/>
-      <c r="V4" s="18">
+      <c r="T4" s="39"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="42">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="W4" s="102"/>
-      <c r="X4" s="103"/>
-      <c r="Y4" s="19">
+      <c r="W4" s="43"/>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="45">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Z4" s="102"/>
-      <c r="AA4" s="103"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="44"/>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B5" s="74"/>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="47">
         <v>3482</v>
       </c>
-      <c r="E5" s="86"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="53">
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="50">
         <v>3291</v>
       </c>
-      <c r="H5" s="86"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="57">
+      <c r="H5" s="48"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="51">
         <v>6027</v>
       </c>
-      <c r="K5" s="92"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="46">
+      <c r="K5" s="52"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="54">
         <v>6721</v>
       </c>
-      <c r="N5" s="92"/>
-      <c r="O5" s="93"/>
-      <c r="P5" s="9">
+      <c r="N5" s="52"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="55">
         <v>225</v>
       </c>
-      <c r="Q5" s="98"/>
-      <c r="R5" s="99"/>
-      <c r="S5" s="60">
+      <c r="Q5" s="56"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="58">
         <v>111</v>
       </c>
-      <c r="T5" s="98"/>
-      <c r="U5" s="99"/>
-      <c r="V5" s="20">
+      <c r="T5" s="56"/>
+      <c r="U5" s="57"/>
+      <c r="V5" s="59">
         <v>3.3E-3</v>
       </c>
-      <c r="W5" s="104"/>
-      <c r="X5" s="105"/>
-      <c r="Y5" s="21">
+      <c r="W5" s="60"/>
+      <c r="X5" s="61"/>
+      <c r="Y5" s="62">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Z5" s="104"/>
-      <c r="AA5" s="105"/>
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="61"/>
     </row>
-    <row r="6" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="73"/>
-      <c r="C6" s="3" t="s">
+    <row r="6" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="15"/>
+      <c r="C6" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="64">
         <v>2830</v>
       </c>
-      <c r="E6" s="88"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="54">
+      <c r="E6" s="65"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="67">
         <v>2985</v>
       </c>
-      <c r="H6" s="88"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="45">
+      <c r="H6" s="65"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="68">
         <v>5810</v>
       </c>
-      <c r="K6" s="94"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="58">
+      <c r="K6" s="69"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="71">
         <v>5267</v>
       </c>
-      <c r="N6" s="94"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="61">
+      <c r="N6" s="69"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="72">
         <v>95</v>
       </c>
-      <c r="Q6" s="100"/>
-      <c r="R6" s="101"/>
-      <c r="S6" s="12">
+      <c r="Q6" s="73"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="75">
         <v>143</v>
       </c>
-      <c r="T6" s="100"/>
-      <c r="U6" s="101"/>
-      <c r="V6" s="22">
+      <c r="T6" s="73"/>
+      <c r="U6" s="74"/>
+      <c r="V6" s="76">
         <v>3.8E-3</v>
       </c>
-      <c r="W6" s="106"/>
-      <c r="X6" s="107"/>
-      <c r="Y6" s="23">
+      <c r="W6" s="77"/>
+      <c r="X6" s="78"/>
+      <c r="Y6" s="79">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="Z6" s="106"/>
-      <c r="AA6" s="107"/>
+      <c r="Z6" s="77"/>
+      <c r="AA6" s="78"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="55">
+      <c r="D7" s="30">
         <v>0.01</v>
       </c>
       <c r="E7" s="33">
         <v>0.02</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="80">
         <v>0.02</v>
       </c>
       <c r="G7" s="33">
         <v>0.02</v>
       </c>
-      <c r="H7" s="68">
+      <c r="H7" s="81">
         <v>0.01</v>
       </c>
-      <c r="I7" s="36">
+      <c r="I7" s="80">
         <v>0.03</v>
       </c>
-      <c r="J7" s="56">
+      <c r="J7" s="34">
         <v>0.03</v>
       </c>
-      <c r="K7" s="44">
+      <c r="K7" s="37">
         <v>0.06</v>
       </c>
-      <c r="L7" s="47">
+      <c r="L7" s="82">
         <v>0.04</v>
       </c>
-      <c r="M7" s="69">
+      <c r="M7" s="83">
         <v>0.03</v>
       </c>
-      <c r="N7" s="44">
+      <c r="N7" s="37">
         <v>0.04</v>
       </c>
-      <c r="O7" s="47">
+      <c r="O7" s="82">
         <v>0.05</v>
       </c>
-      <c r="P7" s="9">
+      <c r="P7" s="55">
         <v>259</v>
       </c>
-      <c r="Q7" s="60">
+      <c r="Q7" s="58">
         <v>66</v>
       </c>
-      <c r="R7" s="64">
+      <c r="R7" s="84">
         <v>220</v>
       </c>
-      <c r="S7" s="63">
+      <c r="S7" s="85">
         <v>83</v>
       </c>
-      <c r="T7" s="10">
+      <c r="T7" s="85">
         <v>80</v>
       </c>
-      <c r="U7" s="13">
+      <c r="U7" s="84">
         <v>69</v>
       </c>
-      <c r="V7" s="18">
+      <c r="V7" s="42">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="W7" s="24">
+      <c r="W7" s="86">
         <v>1.6299999999999999E-2</v>
       </c>
-      <c r="X7" s="25">
+      <c r="X7" s="87">
         <v>5.4000000000000003E-3</v>
       </c>
-      <c r="Y7" s="24">
+      <c r="Y7" s="86">
         <v>1.9E-3</v>
       </c>
-      <c r="Z7" s="24">
+      <c r="Z7" s="86">
         <v>1.35E-2</v>
       </c>
-      <c r="AA7" s="25">
+      <c r="AA7" s="87">
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
     <row r="8" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B8" s="74"/>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="47">
         <v>0.01</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="67">
         <v>0.02</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="88">
         <v>0.01</v>
       </c>
-      <c r="G8" s="35">
+      <c r="G8" s="67">
         <v>0.02</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="67">
         <v>0.02</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="88">
         <v>0.01</v>
       </c>
-      <c r="J8" s="45">
+      <c r="J8" s="68">
         <v>0.03</v>
       </c>
-      <c r="K8" s="46">
+      <c r="K8" s="54">
         <v>0.04</v>
       </c>
-      <c r="L8" s="48">
+      <c r="L8" s="89">
         <v>0.04</v>
       </c>
-      <c r="M8" s="46">
+      <c r="M8" s="54">
         <v>0.04</v>
       </c>
-      <c r="N8" s="46">
+      <c r="N8" s="54">
         <v>0.04</v>
       </c>
-      <c r="O8" s="48">
+      <c r="O8" s="89">
         <v>0.04</v>
       </c>
-      <c r="P8" s="62">
+      <c r="P8" s="90">
         <v>58</v>
       </c>
-      <c r="Q8" s="63">
+      <c r="Q8" s="85">
         <v>64</v>
       </c>
-      <c r="R8" s="64">
+      <c r="R8" s="84">
         <v>79</v>
       </c>
-      <c r="S8" s="10">
+      <c r="S8" s="85">
         <v>64</v>
       </c>
-      <c r="T8" s="10">
+      <c r="T8" s="85">
         <v>64</v>
       </c>
-      <c r="U8" s="13">
+      <c r="U8" s="84">
         <v>81</v>
       </c>
-      <c r="V8" s="22">
+      <c r="V8" s="76">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="W8" s="23">
+      <c r="W8" s="79">
         <v>1.18E-2</v>
       </c>
-      <c r="X8" s="26">
+      <c r="X8" s="91">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="Y8" s="21">
+      <c r="Y8" s="62">
         <v>1E-3</v>
       </c>
-      <c r="Z8" s="23">
+      <c r="Z8" s="79">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="AA8" s="26">
+      <c r="AA8" s="91">
         <v>3.3E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="73"/>
-      <c r="C9" s="3" t="s">
+    <row r="9" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="15"/>
+      <c r="C9" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="92">
         <v>0.01</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="93">
         <v>0.01</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="94">
         <v>0.01</v>
       </c>
-      <c r="G9" s="39">
+      <c r="G9" s="93">
         <v>0.01</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="93">
         <v>0.01</v>
       </c>
-      <c r="I9" s="40">
+      <c r="I9" s="94">
         <v>0.01</v>
       </c>
-      <c r="J9" s="49">
+      <c r="J9" s="95">
         <v>0.03</v>
       </c>
-      <c r="K9" s="50">
+      <c r="K9" s="96">
         <v>0.04</v>
       </c>
-      <c r="L9" s="51">
+      <c r="L9" s="97">
         <v>0.04</v>
       </c>
-      <c r="M9" s="50">
+      <c r="M9" s="96">
         <v>0.03</v>
       </c>
-      <c r="N9" s="50">
+      <c r="N9" s="96">
         <v>0.04</v>
       </c>
-      <c r="O9" s="51">
+      <c r="O9" s="97">
         <v>0.04</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="98">
         <v>324</v>
       </c>
-      <c r="Q9" s="65">
+      <c r="Q9" s="99">
         <v>61</v>
       </c>
-      <c r="R9" s="67">
+      <c r="R9" s="100">
         <v>91</v>
       </c>
-      <c r="S9" s="12">
+      <c r="S9" s="75">
         <v>171</v>
       </c>
-      <c r="T9" s="12">
+      <c r="T9" s="75">
         <v>157</v>
       </c>
-      <c r="U9" s="14">
+      <c r="U9" s="100">
         <v>157</v>
       </c>
-      <c r="V9" s="27">
+      <c r="V9" s="101">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="W9" s="66">
+      <c r="W9" s="102">
         <v>1.4E-2</v>
       </c>
-      <c r="X9" s="29">
+      <c r="X9" s="103">
         <v>3.8E-3</v>
       </c>
-      <c r="Y9" s="28">
+      <c r="Y9" s="104">
         <v>1.8E-3</v>
       </c>
-      <c r="Z9" s="28">
+      <c r="Z9" s="104">
         <v>1.21E-2</v>
       </c>
-      <c r="AA9" s="29">
+      <c r="AA9" s="103">
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
+    <row r="10" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="105" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="106"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="107"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="108"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="27"/>
+      <c r="AA10" s="28"/>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
+    <row r="11" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="109"/>
+      <c r="C11" s="109"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="110"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="111"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
+    <row r="12" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="113" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="14"/>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
+    <row r="13" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="114"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="R13" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="S13" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="T13" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="U13" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="V13" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="W13" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="X13" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y13" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z13" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA13" s="28" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
+      <c r="B14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="39"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="42"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="44"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="43"/>
+      <c r="AA14" s="44"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B15" s="16"/>
+      <c r="C15" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="47"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="57"/>
+      <c r="V15" s="59"/>
+      <c r="W15" s="60"/>
+      <c r="X15" s="61"/>
+      <c r="Y15" s="62"/>
+      <c r="Z15" s="60"/>
+      <c r="AA15" s="61"/>
+    </row>
+    <row r="16" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="15"/>
+      <c r="C16" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="71"/>
+      <c r="N16" s="69"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="72"/>
+      <c r="Q16" s="73"/>
+      <c r="R16" s="74"/>
+      <c r="S16" s="75"/>
+      <c r="T16" s="73"/>
+      <c r="U16" s="74"/>
+      <c r="V16" s="76"/>
+      <c r="W16" s="77"/>
+      <c r="X16" s="78"/>
+      <c r="Y16" s="79"/>
+      <c r="Z16" s="77"/>
+      <c r="AA16" s="78"/>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="82"/>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="84"/>
+      <c r="S17" s="85"/>
+      <c r="T17" s="85"/>
+      <c r="U17" s="84"/>
+      <c r="V17" s="42"/>
+      <c r="W17" s="86"/>
+      <c r="X17" s="87"/>
+      <c r="Y17" s="86"/>
+      <c r="Z17" s="86"/>
+      <c r="AA17" s="87"/>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B18" s="16"/>
+      <c r="C18" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="47"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="88"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="89"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="89"/>
+      <c r="P18" s="90"/>
+      <c r="Q18" s="85"/>
+      <c r="R18" s="84"/>
+      <c r="S18" s="85"/>
+      <c r="T18" s="85"/>
+      <c r="U18" s="84"/>
+      <c r="V18" s="76"/>
+      <c r="W18" s="79"/>
+      <c r="X18" s="91"/>
+      <c r="Y18" s="62"/>
+      <c r="Z18" s="79"/>
+      <c r="AA18" s="91"/>
+    </row>
+    <row r="19" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="15"/>
+      <c r="C19" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="92"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="95"/>
+      <c r="K19" s="96"/>
+      <c r="L19" s="97"/>
+      <c r="M19" s="96"/>
+      <c r="N19" s="96"/>
+      <c r="O19" s="97"/>
+      <c r="P19" s="98"/>
+      <c r="Q19" s="99"/>
+      <c r="R19" s="100"/>
+      <c r="S19" s="75"/>
+      <c r="T19" s="75"/>
+      <c r="U19" s="100"/>
+      <c r="V19" s="101"/>
+      <c r="W19" s="102"/>
+      <c r="X19" s="103"/>
+      <c r="Y19" s="104"/>
+      <c r="Z19" s="104"/>
+      <c r="AA19" s="103"/>
+    </row>
+    <row r="20" spans="2:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="105" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="106"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="107"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="108"/>
+      <c r="X20" s="28"/>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="28"/>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B21" s="112"/>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B22" s="112"/>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B23" s="112"/>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B24" s="112"/>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B25" s="112"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="34">
+    <mergeCell ref="W4:X6"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="V2:AA2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -2217,7 +2649,23 @@
     <mergeCell ref="E4:F6"/>
     <mergeCell ref="K4:L6"/>
     <mergeCell ref="Q4:R6"/>
-    <mergeCell ref="W4:X6"/>
+    <mergeCell ref="P12:U12"/>
+    <mergeCell ref="V12:AA12"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="E14:F16"/>
+    <mergeCell ref="H14:I16"/>
+    <mergeCell ref="K14:L16"/>
+    <mergeCell ref="N14:O16"/>
+    <mergeCell ref="Q14:R16"/>
+    <mergeCell ref="T14:U16"/>
+    <mergeCell ref="W14:X16"/>
+    <mergeCell ref="Z14:AA16"/>
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:I12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>